<commit_message>
minor changes - first day of the testNG
</commit_message>
<xml_diff>
--- a/src/test/resources/inputData/Data.xlsx
+++ b/src/test/resources/inputData/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaiq\eclipse-workspace\com.eagles.datadriven.framework\src\test\resources\inputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\git\testNGFramework\src\test\resources\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7C54A8-B24F-45A8-A0BC-1E997C827D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78114632-C1F7-4FFD-8B62-C3C83E9DBD25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2490" windowWidth="43200" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="3" r:id="rId1"/>
@@ -348,94 +348,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE6E8424-6FA1-4C5F-8DD1-20E60EA41288}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
       </c>
       <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding class code for 1-19-22 - testNG day2
</commit_message>
<xml_diff>
--- a/src/test/resources/inputData/Data.xlsx
+++ b/src/test/resources/inputData/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\git\testNGFramework\src\test\resources\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78114632-C1F7-4FFD-8B62-C3C83E9DBD25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE79AA7C-0D08-4B04-A53F-0F45FA533C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2490" windowWidth="43200" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1065" yWindow="2400" windowWidth="25050" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="3" r:id="rId1"/>
@@ -25,22 +25,82 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>eagles@tekschool.us</t>
   </si>
   <si>
     <t>eagles</t>
+  </si>
+  <si>
+    <t>sample  B 1</t>
+  </si>
+  <si>
+    <t>sample  B 2</t>
+  </si>
+  <si>
+    <t>sample C  1</t>
+  </si>
+  <si>
+    <t>sample C  2</t>
+  </si>
+  <si>
+    <t>sample  B 3</t>
+  </si>
+  <si>
+    <t>sample C  3</t>
+  </si>
+  <si>
+    <t>sample  B 4</t>
+  </si>
+  <si>
+    <t>sample C  4</t>
+  </si>
+  <si>
+    <t>sample  B 5</t>
+  </si>
+  <si>
+    <t>sample C  5</t>
+  </si>
+  <si>
+    <t>sample  B 6</t>
+  </si>
+  <si>
+    <t>sample C  6</t>
+  </si>
+  <si>
+    <t>sample  B 7</t>
+  </si>
+  <si>
+    <t>sample C  7</t>
+  </si>
+  <si>
+    <t>sample  B 8</t>
+  </si>
+  <si>
+    <t>sample C  8</t>
+  </si>
+  <si>
+    <t>sample  B 9</t>
+  </si>
+  <si>
+    <t>sample C  9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -351,12 +411,12 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -375,10 +435,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -386,10 +446,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -397,10 +457,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -408,10 +468,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -419,10 +479,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -430,10 +490,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -441,10 +501,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -452,10 +512,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -463,13 +523,14 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>